<commit_message>
task2 initialization & feedforward
</commit_message>
<xml_diff>
--- a/Dry_Bean_Dataset.xlsx
+++ b/Dry_Bean_Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma elgayar\Desktop\DryBeans\Dry_Bean_Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\college\level 4\1st Semster\NN\perceptron_and_adaline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AC5357-F466-42A4-8663-E01C7C926EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EB7560-F193-438A-AC5C-17CAF139E300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dry_Beans_Dataset" sheetId="1" r:id="rId1"/>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>